<commit_message>
Changement d'ordre des couleurs
</commit_message>
<xml_diff>
--- a/serveur/PokerServer_début/cartes.xlsx
+++ b/serveur/PokerServer_début/cartes.xlsx
@@ -33,15 +33,9 @@
     <t>AS de pique</t>
   </si>
   <si>
-    <t>AS de carreaux</t>
-  </si>
-  <si>
     <t>AS de trefle</t>
   </si>
   <si>
-    <t>As de cœur</t>
-  </si>
-  <si>
     <t>2 de pique</t>
   </si>
   <si>
@@ -55,6 +49,12 @@
   </si>
   <si>
     <t>etc</t>
+  </si>
+  <si>
+    <t>AS de cœur</t>
+  </si>
+  <si>
+    <t>As de carreaux</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -468,7 +468,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -482,7 +482,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -510,7 +510,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -664,10 +664,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>21</v>

</xml_diff>